<commit_message>
Changed project to Maven management
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="v0.0.1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Input</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -34,86 +32,15 @@
   </si>
   <si>
     <t>Req.</t>
-  </si>
-  <si>
-    <t>The application checks for 'data.json'</t>
-  </si>
-  <si>
-    <t>Application has just loaded</t>
   </si>
   <si>
     <t>Expected
 Results</t>
   </si>
   <si>
-    <t>Actual
-Results</t>
-  </si>
-  <si>
-    <t>The application accurately identifies whether 'data.json' exists</t>
-  </si>
-  <si>
-    <t>The application asks the user for the full name of new character</t>
-  </si>
-  <si>
     <t>The application finds the character folder using the full name given by the user</t>
   </si>
   <si>
-    <r>
-      <t>There are unidentified character folders in the user directory (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>excluding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the folder for the character given by the user)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>There are unidentified character folders in the user directory (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>including</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the folder for the character given by the user)</t>
-    </r>
-  </si>
-  <si>
-    <t>The application indicates that the given character was not found in the user folder</t>
-  </si>
-  <si>
     <t>1.2.1.2.1</t>
   </si>
   <si>
@@ -145,13 +72,94 @@
   </si>
   <si>
     <t>When backups are made, (in-game) changes made by the user to components will affect their respective profiles</t>
+  </si>
+  <si>
+    <t>Pre-Condition</t>
+  </si>
+  <si>
+    <t>Application is initializing</t>
+  </si>
+  <si>
+    <t>The application finds the character when there is only one instance</t>
+  </si>
+  <si>
+    <t>The 'data.json' file exists.</t>
+  </si>
+  <si>
+    <t>The application aggregates Java-object data using the entries in the JSON file.</t>
+  </si>
+  <si>
+    <t>The 'data.json' file does not exist.</t>
+  </si>
+  <si>
+    <t>The application begins asking the user for character names.</t>
+  </si>
+  <si>
+    <t>The application is asking the user for the name of a character to identify.
+There is at least one unidentified character whose name is unique among all other characters.</t>
+  </si>
+  <si>
+    <t>The user inputs the name of a unique character.</t>
+  </si>
+  <si>
+    <t>The application finds the character when there is more than one instance</t>
+  </si>
+  <si>
+    <t>The application is asking the user for the name of a character to identify.
+There is at least one unidentified character whose name is shared with another character.</t>
+  </si>
+  <si>
+    <t>The user inputs the name of a non-unique character.</t>
+  </si>
+  <si>
+    <t>The application identifies the duplicate characters and lists their World names.
+The application finds the character folder using the full name given by the user</t>
+  </si>
+  <si>
+    <t>The application identifies the World  names when more than  one character is identified using a given name</t>
+  </si>
+  <si>
+    <t>The application has listed the two or more Worlds that the character has been found in.</t>
+  </si>
+  <si>
+    <t>The user confirms that the list of Worlds accurately reflects their characters'  locations.</t>
+  </si>
+  <si>
+    <t>The application adds all characters found with the duplicate name, to their respective Worlds.</t>
+  </si>
+  <si>
+    <t>The application displays an error when an  character cannot be found.</t>
+  </si>
+  <si>
+    <t>The application displays an error when an  invalid character name has been.</t>
+  </si>
+  <si>
+    <t>The application is asking the user for the name of a character to identify.</t>
+  </si>
+  <si>
+    <t>The user enters a name that does not follow FFXIV's naming convention</t>
+  </si>
+  <si>
+    <t>The user enters the name of a character that does not exist in their user folder</t>
+  </si>
+  <si>
+    <t>The application displays a warning message indicating that the character could not be found</t>
+  </si>
+  <si>
+    <t>The application displays a warning message about the invalid name entry.</t>
+  </si>
+  <si>
+    <t>Handling 'data.json'</t>
+  </si>
+  <si>
+    <t>Handling non-existent 'data.json'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,14 +175,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -192,22 +192,209 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -216,9 +403,80 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -267,7 +525,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,9 +558,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,6 +610,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,146 +803,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="19" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +1045,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -677,7 +1057,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>